<commit_message>
Generate graph from resulted cluster
</commit_message>
<xml_diff>
--- a/Graph.xlsx
+++ b/Graph.xlsx
@@ -16,9 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Number of Sequence</t>
+  </si>
+  <si>
+    <t>Number of Cluster</t>
+  </si>
+  <si>
+    <t>Threshold</t>
   </si>
 </sst>
 </file>
@@ -42,7 +48,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +56,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,9 +94,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -314,11 +337,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="71150592"/>
-        <c:axId val="71267072"/>
+        <c:axId val="232986112"/>
+        <c:axId val="232987648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71150592"/>
+        <c:axId val="232986112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,14 +349,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71267072"/>
+        <c:crossAx val="232987648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71267072"/>
+        <c:axId val="232987648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -342,20 +365,19 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71150592"/>
+        <c:crossAx val="232986112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -364,6 +386,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -375,7 +398,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
+              <c:f>Sheet2!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -389,7 +412,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -437,7 +460,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$14</c:f>
+              <c:f>Sheet2!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -489,7 +512,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$1</c:f>
+              <c:f>Sheet2!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -503,7 +526,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -551,7 +574,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$14</c:f>
+              <c:f>Sheet2!$C$4:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -603,7 +626,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>Sheet2!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -617,7 +640,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -665,7 +688,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$14</c:f>
+              <c:f>Sheet2!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -717,7 +740,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$1</c:f>
+              <c:f>Sheet2!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -731,7 +754,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -779,7 +802,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$E$2:$E$14</c:f>
+              <c:f>Sheet2!$E$4:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -831,7 +854,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$F$1</c:f>
+              <c:f>Sheet2!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -845,7 +868,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -893,7 +916,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$F$2:$F$14</c:f>
+              <c:f>Sheet2!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -945,7 +968,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$1</c:f>
+              <c:f>Sheet2!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -959,7 +982,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1007,7 +1030,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$2:$G$14</c:f>
+              <c:f>Sheet2!$G$4:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1059,7 +1082,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$H$1</c:f>
+              <c:f>Sheet2!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1073,7 +1096,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1121,7 +1144,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$H$2:$H$14</c:f>
+              <c:f>Sheet2!$H$4:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1173,7 +1196,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$I$1</c:f>
+              <c:f>Sheet2!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1187,7 +1210,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1235,7 +1258,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$I$2:$I$14</c:f>
+              <c:f>Sheet2!$I$4:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1287,7 +1310,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$J$1</c:f>
+              <c:f>Sheet2!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1301,7 +1324,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1349,7 +1372,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$J$2:$J$14</c:f>
+              <c:f>Sheet2!$J$4:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1401,7 +1424,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$K$1</c:f>
+              <c:f>Sheet2!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1415,7 +1438,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1463,7 +1486,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$K$2:$K$14</c:f>
+              <c:f>Sheet2!$K$4:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1515,7 +1538,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$L$1</c:f>
+              <c:f>Sheet2!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1529,7 +1552,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1577,7 +1600,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$L$2:$L$14</c:f>
+              <c:f>Sheet2!$L$4:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1629,7 +1652,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$M$1</c:f>
+              <c:f>Sheet2!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1643,7 +1666,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$14</c:f>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1691,7 +1714,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$M$2:$M$14</c:f>
+              <c:f>Sheet2!$M$4:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1738,13 +1761,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="93160192"/>
-        <c:axId val="93162880"/>
+        <c:axId val="232949632"/>
+        <c:axId val="232968192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93160192"/>
+        <c:axId val="232949632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1797,14 +1819,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93162880"/>
+        <c:crossAx val="232968192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93162880"/>
+        <c:axId val="232968192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1845,7 +1867,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93160192"/>
+        <c:crossAx val="232949632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1856,9 +1878,12 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:ln w="25400"/>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1905,13 +1930,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2401,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A2:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M14"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2412,583 +2437,606 @@
     <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
         <v>0.05</v>
       </c>
-      <c r="C1">
+      <c r="C2" s="1">
         <v>0.1</v>
       </c>
-      <c r="D1">
+      <c r="D2" s="1">
         <v>0.2</v>
       </c>
-      <c r="E1">
+      <c r="E2" s="1">
         <v>0.3</v>
       </c>
-      <c r="F1">
+      <c r="F2" s="1">
         <v>0.4</v>
       </c>
-      <c r="G1">
+      <c r="G2" s="1">
         <v>0.5</v>
       </c>
-      <c r="H1">
+      <c r="H2" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I1">
+      <c r="I2" s="1">
         <v>0.6</v>
       </c>
-      <c r="J1">
+      <c r="J2" s="1">
         <v>0.7</v>
       </c>
-      <c r="K1">
+      <c r="K2" s="1">
         <v>0.8</v>
       </c>
-      <c r="L1">
+      <c r="L2" s="1">
         <v>0.9</v>
       </c>
-      <c r="M1">
+      <c r="M2" s="1">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
-      <c r="M2">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3">
-        <v>5</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3">
-        <v>5</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>6</v>
-      </c>
-      <c r="L4">
-        <v>6</v>
-      </c>
-      <c r="M4">
-        <v>6</v>
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="J5">
-        <v>7</v>
-      </c>
-      <c r="K5">
-        <v>7</v>
-      </c>
-      <c r="L5">
-        <v>7</v>
-      </c>
-      <c r="M5">
-        <v>7</v>
+      <c r="A5" s="1">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
+      <c r="A6" s="1">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1">
         <v>8</v>
       </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6">
-        <v>7</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
-      </c>
-      <c r="K6">
-        <v>7</v>
-      </c>
-      <c r="L6">
-        <v>7</v>
-      </c>
-      <c r="M6">
-        <v>7</v>
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1">
+        <v>6</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7">
-        <v>60</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="1">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>8</v>
       </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>7</v>
-      </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <v>7</v>
-      </c>
-      <c r="K7">
-        <v>7</v>
-      </c>
-      <c r="L7">
-        <v>7</v>
-      </c>
-      <c r="M7">
+      <c r="E7" s="1">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1">
+        <v>7</v>
+      </c>
+      <c r="L7" s="1">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8">
-        <v>70</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="1">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
         <v>8</v>
       </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8">
-        <v>7</v>
-      </c>
-      <c r="K8">
-        <v>7</v>
-      </c>
-      <c r="L8">
-        <v>7</v>
-      </c>
-      <c r="M8">
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7</v>
+      </c>
+      <c r="L8" s="1">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9">
-        <v>80</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
+      <c r="A9" s="1">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>7</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9">
-        <v>7</v>
-      </c>
-      <c r="J9">
-        <v>7</v>
-      </c>
-      <c r="K9">
-        <v>7</v>
-      </c>
-      <c r="L9">
-        <v>7</v>
-      </c>
-      <c r="M9">
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1">
+        <v>7</v>
+      </c>
+      <c r="K9" s="1">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1">
+        <v>7</v>
+      </c>
+      <c r="M9" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10">
-        <v>90</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="1">
+        <v>70</v>
+      </c>
+      <c r="B10" s="1">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>8</v>
       </c>
-      <c r="E10">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>7</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>7</v>
-      </c>
-      <c r="K10">
-        <v>7</v>
-      </c>
-      <c r="L10">
-        <v>7</v>
-      </c>
-      <c r="M10">
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1">
+        <v>7</v>
+      </c>
+      <c r="K10" s="1">
+        <v>7</v>
+      </c>
+      <c r="L10" s="1">
+        <v>7</v>
+      </c>
+      <c r="M10" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11">
-        <v>100</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="1">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>8</v>
       </c>
-      <c r="E11">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>7</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11">
-        <v>7</v>
-      </c>
-      <c r="J11">
-        <v>7</v>
-      </c>
-      <c r="K11">
-        <v>7</v>
-      </c>
-      <c r="L11">
-        <v>7</v>
-      </c>
-      <c r="M11">
+      <c r="E11" s="1">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1">
+        <v>7</v>
+      </c>
+      <c r="K11" s="1">
+        <v>7</v>
+      </c>
+      <c r="L11" s="1">
+        <v>7</v>
+      </c>
+      <c r="M11" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="1">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>8</v>
       </c>
-      <c r="E12">
-        <v>7</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
-      <c r="G12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
-      <c r="J12">
-        <v>7</v>
-      </c>
-      <c r="K12">
-        <v>7</v>
-      </c>
-      <c r="L12">
-        <v>7</v>
-      </c>
-      <c r="M12">
+      <c r="E12" s="1">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7</v>
+      </c>
+      <c r="H12" s="1">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1">
+        <v>7</v>
+      </c>
+      <c r="J12" s="1">
+        <v>7</v>
+      </c>
+      <c r="K12" s="1">
+        <v>7</v>
+      </c>
+      <c r="L12" s="1">
+        <v>7</v>
+      </c>
+      <c r="M12" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13">
-        <v>120</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="1">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>10</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>8</v>
       </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>7</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
-      <c r="H13">
-        <v>7</v>
-      </c>
-      <c r="I13">
-        <v>7</v>
-      </c>
-      <c r="J13">
-        <v>7</v>
-      </c>
-      <c r="K13">
-        <v>7</v>
-      </c>
-      <c r="L13">
-        <v>7</v>
-      </c>
-      <c r="M13">
+      <c r="E13" s="1">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1">
+        <v>7</v>
+      </c>
+      <c r="H13" s="1">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1">
+        <v>7</v>
+      </c>
+      <c r="K13" s="1">
+        <v>7</v>
+      </c>
+      <c r="L13" s="1">
+        <v>7</v>
+      </c>
+      <c r="M13" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14">
+      <c r="A14" s="1">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1">
+        <v>7</v>
+      </c>
+      <c r="I14" s="1">
+        <v>7</v>
+      </c>
+      <c r="J14" s="1">
+        <v>7</v>
+      </c>
+      <c r="K14" s="1">
+        <v>7</v>
+      </c>
+      <c r="L14" s="1">
+        <v>7</v>
+      </c>
+      <c r="M14" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1">
+        <v>120</v>
+      </c>
+      <c r="B15" s="1">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7</v>
+      </c>
+      <c r="G15" s="1">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1">
+        <v>7</v>
+      </c>
+      <c r="I15" s="1">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7</v>
+      </c>
+      <c r="K15" s="1">
+        <v>7</v>
+      </c>
+      <c r="L15" s="1">
+        <v>7</v>
+      </c>
+      <c r="M15" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1">
         <v>127</v>
       </c>
-      <c r="B14">
+      <c r="B16" s="1">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C16" s="1">
         <v>12</v>
       </c>
-      <c r="D14">
+      <c r="D16" s="1">
         <v>8</v>
       </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
-      <c r="G14">
-        <v>7</v>
-      </c>
-      <c r="H14">
-        <v>7</v>
-      </c>
-      <c r="I14">
-        <v>7</v>
-      </c>
-      <c r="J14">
-        <v>7</v>
-      </c>
-      <c r="K14">
-        <v>7</v>
-      </c>
-      <c r="L14">
-        <v>7</v>
-      </c>
-      <c r="M14">
+      <c r="E16" s="1">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1">
+        <v>7</v>
+      </c>
+      <c r="K16" s="1">
+        <v>7</v>
+      </c>
+      <c r="L16" s="1">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:M3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Generate graph from resulted clusters
</commit_message>
<xml_diff>
--- a/Graph.xlsx
+++ b/Graph.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Number of Sequence</t>
   </si>
@@ -93,312 +91,45 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Implementation of Algorithm Rata </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Comparison of Threshold Value</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>127</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showVal val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>127</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showVal val="1"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:axId val="232986112"/>
-        <c:axId val="232987648"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="232986112"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232987648"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="232987648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232986112"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$B$2</c:f>
+              <c:f>Sheet3!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -412,7 +143,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -460,7 +191,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$4:$B$16</c:f>
+              <c:f>Sheet3!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -468,51 +199,51 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$2</c:f>
+              <c:f>Sheet3!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -526,7 +257,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -574,7 +305,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$4:$C$16</c:f>
+              <c:f>Sheet3!$C$4:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -582,51 +313,51 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$2</c:f>
+              <c:f>Sheet3!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -640,7 +371,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -688,7 +419,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$4:$D$16</c:f>
+              <c:f>Sheet3!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -696,51 +427,51 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$2</c:f>
+              <c:f>Sheet3!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -754,7 +485,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -802,7 +533,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$E$4:$E$16</c:f>
+              <c:f>Sheet3!$E$4:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -825,36 +556,36 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$F$2</c:f>
+              <c:f>Sheet3!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -868,7 +599,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -916,7 +647,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$F$4:$F$16</c:f>
+              <c:f>Sheet3!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -939,36 +670,36 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$2</c:f>
+              <c:f>Sheet3!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -982,7 +713,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1030,7 +761,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$4:$G$16</c:f>
+              <c:f>Sheet3!$G$4:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1053,25 +784,140 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="8"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$H$4:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1079,14 +925,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="6"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$H$2</c:f>
+              <c:f>Sheet3!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1096,7 +942,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1144,27 +990,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$H$4:$H$16</c:f>
+              <c:f>Sheet3!$I$4:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
@@ -1173,19 +1019,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1193,14 +1039,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="7"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$I$2</c:f>
+              <c:f>Sheet3!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1210,7 +1056,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1258,7 +1104,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$I$4:$I$16</c:f>
+              <c:f>Sheet3!$J$4:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1266,19 +1112,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
@@ -1287,19 +1133,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1307,14 +1153,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
-          <c:order val="8"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$J$2</c:f>
+              <c:f>Sheet3!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1324,7 +1170,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1372,7 +1218,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$J$4:$J$16</c:f>
+              <c:f>Sheet3!$K$4:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1380,19 +1226,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
@@ -1401,19 +1247,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1421,14 +1267,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
-          <c:order val="9"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$K$2</c:f>
+              <c:f>Sheet3!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1438,7 +1284,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1486,7 +1332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$K$4:$K$16</c:f>
+              <c:f>Sheet3!$L$4:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1494,19 +1340,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
@@ -1515,19 +1361,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1535,14 +1381,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
-          <c:order val="10"/>
+          <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$L$2</c:f>
+              <c:f>Sheet3!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1552,7 +1398,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:f>Sheet3!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1600,7 +1446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$L$4:$L$16</c:f>
+              <c:f>Sheet3!$M$4:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1608,19 +1454,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
@@ -1629,144 +1475,31 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="12"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$M$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet2!$A$4:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>127</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$M$4:$M$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="232949632"/>
-        <c:axId val="232968192"/>
+        <c:axId val="46486656"/>
+        <c:axId val="46488192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="232949632"/>
+        <c:axId val="46486656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,29 +1511,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800">
-                    <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
+                  <a:defRPr sz="2400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800">
-                    <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>Number</a:t>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Number of Sequences</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800" baseline="0">
-                    <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> of Sequences</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1800">
-                  <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                  <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1814,19 +1530,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1"/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232968192"/>
+        <c:crossAx val="46488192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232968192"/>
+        <c:axId val="46488192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1838,16 +1554,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800">
-                    <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
+                  <a:defRPr sz="2400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800">
-                    <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US" sz="2400"/>
                   <a:t>Number of Clusters</a:t>
                 </a:r>
               </a:p>
@@ -1862,12 +1572,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1"/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232949632"/>
+        <c:crossAx val="46486656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1875,15 +1585,29 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:spPr>
-    <a:ln w="25400"/>
+    <a:ln w="12700" cap="rnd">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+    </a:ln>
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1893,55 +1617,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2244,198 +1933,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A2:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1">
-        <v>0.05</v>
-      </c>
-      <c r="C1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.05</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>50</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>60</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>70</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>80</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>90</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>100</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>110</v>
-      </c>
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>120</v>
-      </c>
-      <c r="B14">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>127</v>
-      </c>
-      <c r="B15">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:M16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
@@ -2543,13 +2047,13 @@
         <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
@@ -2567,16 +2071,16 @@
         <v>5</v>
       </c>
       <c r="J5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2584,13 +2088,13 @@
         <v>30</v>
       </c>
       <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
         <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>7</v>
       </c>
       <c r="E6" s="1">
         <v>6</v>
@@ -2605,19 +2109,19 @@
         <v>6</v>
       </c>
       <c r="I6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2625,13 +2129,13 @@
         <v>40</v>
       </c>
       <c r="B7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>7</v>
@@ -2646,19 +2150,19 @@
         <v>7</v>
       </c>
       <c r="I7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2666,13 +2170,13 @@
         <v>50</v>
       </c>
       <c r="B8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1">
         <v>7</v>
@@ -2687,19 +2191,19 @@
         <v>7</v>
       </c>
       <c r="I8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2707,13 +2211,13 @@
         <v>60</v>
       </c>
       <c r="B9" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
         <v>7</v>
@@ -2728,19 +2232,19 @@
         <v>7</v>
       </c>
       <c r="I9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2748,25 +2252,25 @@
         <v>70</v>
       </c>
       <c r="B10" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1">
         <v>8</v>
       </c>
-      <c r="E10" s="1">
-        <v>7</v>
-      </c>
       <c r="F10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I10" s="1">
         <v>7</v>
@@ -2789,25 +2293,25 @@
         <v>80</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1">
         <v>8</v>
       </c>
-      <c r="E11" s="1">
-        <v>7</v>
-      </c>
       <c r="F11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I11" s="1">
         <v>7</v>
@@ -2830,40 +2334,40 @@
         <v>90</v>
       </c>
       <c r="B12" s="1">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
+      <c r="F12" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="1">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>7</v>
-      </c>
       <c r="G12" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H12" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2871,40 +2375,40 @@
         <v>100</v>
       </c>
       <c r="B13" s="1">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1">
         <v>10</v>
       </c>
-      <c r="C13" s="1">
+      <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="D13" s="1">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>7</v>
-      </c>
       <c r="G13" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H13" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M13" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -2912,40 +2416,40 @@
         <v>110</v>
       </c>
       <c r="B14" s="1">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
         <v>10</v>
       </c>
-      <c r="C14" s="1">
+      <c r="F14" s="1">
         <v>10</v>
       </c>
-      <c r="D14" s="1">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1">
-        <v>7</v>
-      </c>
-      <c r="F14" s="1">
-        <v>7</v>
-      </c>
       <c r="G14" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H14" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J14" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K14" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L14" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M14" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -2953,40 +2457,40 @@
         <v>120</v>
       </c>
       <c r="B15" s="1">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
         <v>10</v>
       </c>
-      <c r="C15" s="1">
+      <c r="F15" s="1">
         <v>10</v>
       </c>
-      <c r="D15" s="1">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1">
-        <v>7</v>
-      </c>
       <c r="G15" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H15" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I15" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J15" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K15" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L15" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M15" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -2994,40 +2498,40 @@
         <v>127</v>
       </c>
       <c r="B16" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H16" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I16" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J16" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K16" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L16" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M16" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3035,19 +2539,6 @@
     <mergeCell ref="B3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>